<commit_message>
a bnch of xlsx and pngs
</commit_message>
<xml_diff>
--- a/linear_regressions/thread_size/author_threshold/books_regression_metrics.xlsx
+++ b/linear_regressions/thread_size/author_threshold/books_regression_metrics.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snuzz\Documents\PhD\datasets\reddit_analyses\reddit_analyses\linear_regressions\thread_size\author_threshold\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C02AB9-A1AA-42D2-91CE-CD3BFA7F3F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,20 @@
     <sheet name="p1_mod7" sheetId="11" r:id="rId11"/>
     <sheet name="p1_mod8" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -267,8 +286,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,8 +339,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -331,13 +353,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -375,7 +405,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -409,6 +439,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -443,9 +474,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -618,14 +650,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -633,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -641,7 +679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -649,7 +687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -657,7 +695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -665,7 +703,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -673,7 +711,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -681,7 +719,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -689,7 +727,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -697,7 +735,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -705,7 +743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -713,7 +751,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -721,7 +759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -729,7 +767,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -743,14 +781,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -761,7 +799,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
@@ -769,94 +807,94 @@
         <v>3.07759658232334</v>
       </c>
       <c r="C2">
-        <v>0.5686018202853224</v>
+        <v>0.56860182028532236</v>
       </c>
       <c r="D2">
-        <v>3.891462617264311E-07</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>3.8914626172643108E-7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B3">
-        <v>-0.02872145981904009</v>
+        <v>-2.872145981904009E-2</v>
       </c>
       <c r="C3">
-        <v>0.02019827796089082</v>
+        <v>2.0198277960890819E-2</v>
       </c>
       <c r="D3">
         <v>0.1579691152896574</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B4">
-        <v>-0.04037077590210206</v>
+        <v>-4.0370775902102057E-2</v>
       </c>
       <c r="C4">
-        <v>0.06210290649109308</v>
+        <v>6.2102906491093082E-2</v>
       </c>
       <c r="D4">
-        <v>0.5170581772905417</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>0.51705817729054171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B5">
-        <v>-0.5524326712158678</v>
+        <v>-0.55243267121586781</v>
       </c>
       <c r="C5">
         <v>0.1795412465733611</v>
       </c>
       <c r="D5">
-        <v>0.00266190839536768</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>2.6619083953676802E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B6">
-        <v>-0.1382584596039252</v>
+        <v>-0.13825845960392519</v>
       </c>
       <c r="C6">
-        <v>0.1943120992854306</v>
+        <v>0.19431209928543061</v>
       </c>
       <c r="D6">
         <v>0.4783201767408426</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B7">
-        <v>0.5237020984732714</v>
+        <v>0.52370209847327143</v>
       </c>
       <c r="C7">
-        <v>1.059074636679281</v>
+        <v>1.0590746366792809</v>
       </c>
       <c r="D7">
         <v>0.6219832749141978</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B8">
-        <v>0.1754916390542819</v>
+        <v>0.17549163905428189</v>
       </c>
       <c r="C8">
         <v>0.197090932863453</v>
       </c>
       <c r="D8">
-        <v>0.3752625469374085</v>
+        <v>0.37526254693740851</v>
       </c>
     </row>
   </sheetData>
@@ -865,14 +903,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -883,116 +921,116 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B2">
-        <v>3.081374847181842</v>
+        <v>3.0813748471818418</v>
       </c>
       <c r="C2">
-        <v>0.5706240452680698</v>
+        <v>0.57062404526806976</v>
       </c>
       <c r="D2">
-        <v>4.172251484422613E-07</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>4.1722514844226133E-7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B3">
-        <v>-0.09411729670773336</v>
+        <v>-9.4117296707733361E-2</v>
       </c>
       <c r="C3">
-        <v>0.182043387744676</v>
+        <v>0.18204338774467599</v>
       </c>
       <c r="D3">
-        <v>0.6062401805117645</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.60624018051176454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B4">
-        <v>-0.0298302646092516</v>
+        <v>-2.9830264609251599E-2</v>
       </c>
       <c r="C4">
-        <v>0.02038160187791932</v>
+        <v>2.038160187791932E-2</v>
       </c>
       <c r="D4">
-        <v>0.1462938814487905</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>0.14629388144879049</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B5">
-        <v>-0.03967484872214411</v>
+        <v>-3.9674848722144107E-2</v>
       </c>
       <c r="C5">
-        <v>0.06233319913002097</v>
+        <v>6.2333199130020972E-2</v>
       </c>
       <c r="D5">
-        <v>0.5258381473277257</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>0.52583814732772571</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B6">
-        <v>-0.5577857914963766</v>
+        <v>-0.55778579149637664</v>
       </c>
       <c r="C6">
-        <v>0.180462286019145</v>
+        <v>0.18046228601914499</v>
       </c>
       <c r="D6">
-        <v>0.002555482764647417</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>2.555482764647417E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B7">
-        <v>-0.1484590568526185</v>
+        <v>-0.14845905685261851</v>
       </c>
       <c r="C7">
-        <v>0.1959828523558967</v>
+        <v>0.19598285235589669</v>
       </c>
       <c r="D7">
-        <v>0.4504407695616617</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>0.45044076956166168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B8">
-        <v>0.5639208119589021</v>
+        <v>0.56392081195890209</v>
       </c>
       <c r="C8">
-        <v>1.065597363136049</v>
+        <v>1.0655973631360489</v>
       </c>
       <c r="D8">
-        <v>0.5977794041936498</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>0.59777940419364983</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B9">
-        <v>0.1853464087352983</v>
+        <v>0.18534640873529831</v>
       </c>
       <c r="C9">
         <v>0.1986920857590577</v>
       </c>
       <c r="D9">
-        <v>0.3530466244278261</v>
+        <v>0.35304662442782608</v>
       </c>
     </row>
   </sheetData>
@@ -1001,14 +1039,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1019,7 +1057,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
@@ -1027,27 +1065,27 @@
         <v>3.088355429701235</v>
       </c>
       <c r="C2">
-        <v>0.5734869292173889</v>
+        <v>0.57348692921738886</v>
       </c>
       <c r="D2">
-        <v>4.516535976452903E-07</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>4.5165359764529032E-7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B3">
-        <v>-0.09052678204499089</v>
+        <v>-9.0526782044990886E-2</v>
       </c>
       <c r="C3">
-        <v>0.1831662097425446</v>
+        <v>0.18316620974254461</v>
       </c>
       <c r="D3">
-        <v>0.6221839711394525</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.62218397113945245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>78</v>
       </c>
@@ -1055,83 +1093,83 @@
         <v>-0.1802402083458064</v>
       </c>
       <c r="C4">
-        <v>0.560461799566108</v>
+        <v>0.56046179956610798</v>
       </c>
       <c r="D4">
-        <v>0.7484070178167124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>0.74840701781671237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B5">
-        <v>-0.03047077171288599</v>
+        <v>-3.047077171288599E-2</v>
       </c>
       <c r="C5">
-        <v>0.02056584857975742</v>
+        <v>2.056584857975742E-2</v>
       </c>
       <c r="D5">
         <v>0.1414650370729533</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B6">
-        <v>-0.03698740993451282</v>
+        <v>-3.698740993451282E-2</v>
       </c>
       <c r="C6">
-        <v>0.06315634825733368</v>
+        <v>6.3156348257333683E-2</v>
       </c>
       <c r="D6">
-        <v>0.5593805931935742</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>0.55938059319357425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B7">
-        <v>-0.5410507408831052</v>
+        <v>-0.54105074088310523</v>
       </c>
       <c r="C7">
-        <v>0.1885605367398593</v>
+        <v>0.18856053673985931</v>
       </c>
       <c r="D7">
-        <v>0.004982204771140327</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>4.9822047711403266E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B8">
-        <v>-0.1423180293501445</v>
+        <v>-0.14231802935014451</v>
       </c>
       <c r="C8">
-        <v>0.1977491319607863</v>
+        <v>0.19774913196078631</v>
       </c>
       <c r="D8">
-        <v>0.4733302506243198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>0.47333025062431983</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B9">
-        <v>0.5635660621167026</v>
+        <v>0.56356606211670257</v>
       </c>
       <c r="C9">
-        <v>1.070176759647454</v>
+        <v>1.0701767596474541</v>
       </c>
       <c r="D9">
-        <v>0.5995856346221382</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>0.59958563462213821</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -1142,7 +1180,7 @@
         <v>0.2016744291055807</v>
       </c>
       <c r="D10">
-        <v>0.3364653553666043</v>
+        <v>0.33646535536660432</v>
       </c>
     </row>
   </sheetData>
@@ -1151,14 +1189,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1178,7 +1219,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1192,13 +1233,13 @@
         <v>37</v>
       </c>
       <c r="E2">
-        <v>0.09344660077359113</v>
+        <v>9.3446600773591126E-2</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1218,7 +1259,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1238,7 +1279,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1258,7 +1299,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1278,7 +1319,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1292,13 +1333,13 @@
         <v>42</v>
       </c>
       <c r="E7">
-        <v>0.1237498944355828</v>
+        <v>0.12374989443558281</v>
       </c>
       <c r="F7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1318,7 +1359,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1332,7 +1373,7 @@
         <v>44</v>
       </c>
       <c r="E9">
-        <v>0.1268431629522195</v>
+        <v>0.12684316295221951</v>
       </c>
       <c r="F9" t="s">
         <v>52</v>
@@ -1344,14 +1385,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -1365,7 +1412,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1373,13 +1420,13 @@
         <v>56</v>
       </c>
       <c r="C2">
-        <v>0.0934466007735909</v>
+        <v>9.3446600773590904E-2</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1393,7 +1440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1407,7 +1454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1421,7 +1468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1435,7 +1482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1449,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1463,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1471,9 +1518,19 @@
         <v>63</v>
       </c>
       <c r="C9">
-        <v>0.1268431629522196</v>
+        <v>0.12684316295221959</v>
       </c>
       <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f>MAX(C2:C9)</f>
+        <v>0.12684316295221959</v>
+      </c>
+      <c r="D13">
+        <f>MAX(D2:D9)</f>
         <v>0</v>
       </c>
     </row>
@@ -1483,14 +1540,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1504,8 +1563,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1518,8 +1577,8 @@
         <v>757</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>67</v>
       </c>
@@ -1528,6 +1587,12 @@
       </c>
       <c r="D3">
         <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f>SUM(D2:D3)</f>
+        <v>1037</v>
       </c>
     </row>
   </sheetData>
@@ -1539,14 +1604,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1557,32 +1622,32 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B2">
-        <v>2.899123314146819</v>
+        <v>2.8991233141468191</v>
       </c>
       <c r="C2">
-        <v>0.1377731710045929</v>
+        <v>0.13777317100459291</v>
       </c>
       <c r="D2">
-        <v>1.532530016840004E-40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>1.5325300168400039E-40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B3">
-        <v>-0.5620523598854335</v>
+        <v>-0.56205235988543345</v>
       </c>
       <c r="C3">
-        <v>0.1661614324582528</v>
+        <v>0.16616143245825279</v>
       </c>
       <c r="D3">
-        <v>0.0009926893357968356</v>
+        <v>9.9268933579683559E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1591,14 +1656,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1609,12 +1674,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B2">
-        <v>3.240342881387685</v>
+        <v>3.2403428813876851</v>
       </c>
       <c r="C2">
         <v>0.2682709434141155</v>
@@ -1623,32 +1688,32 @@
         <v>6.804097232743109E-22</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B3">
-        <v>-0.02897201104954995</v>
+        <v>-2.897201104954995E-2</v>
       </c>
       <c r="C3">
-        <v>0.01958193995181843</v>
+        <v>1.9581939951818429E-2</v>
       </c>
       <c r="D3">
-        <v>0.141857717922601</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.14185771792260099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B4">
-        <v>-0.5277655662427674</v>
+        <v>-0.52776556624276738</v>
       </c>
       <c r="C4">
-        <v>0.1668953299042465</v>
+        <v>0.16689532990424649</v>
       </c>
       <c r="D4">
-        <v>0.002023573426409396</v>
+        <v>2.0235734264093959E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1657,14 +1722,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1675,54 +1740,54 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B2">
-        <v>2.985598025745966</v>
+        <v>2.9855980257459662</v>
       </c>
       <c r="C2">
-        <v>0.4342520198192406</v>
+        <v>0.43425201981924061</v>
       </c>
       <c r="D2">
-        <v>4.044895299436245E-10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>4.0448952994362448E-10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B3">
-        <v>-0.02827676845507282</v>
+        <v>-2.827676845507282E-2</v>
       </c>
       <c r="C3">
-        <v>0.01964347214030657</v>
+        <v>1.9643472140306571E-2</v>
       </c>
       <c r="D3">
-        <v>0.1528747850606736</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.15287478506067359</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B4">
-        <v>-0.521509857315778</v>
+        <v>-0.52150985731577804</v>
       </c>
       <c r="C4">
         <v>0.16744129382699</v>
       </c>
       <c r="D4">
-        <v>0.002353983422309758</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>2.3539834223097579E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B5">
-        <v>0.1355753993747238</v>
+        <v>0.13557539937472379</v>
       </c>
       <c r="C5">
         <v>0.1815070702169515</v>
@@ -1737,14 +1802,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1755,63 +1820,63 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B2">
-        <v>3.148250455515409</v>
+        <v>3.1482504555154089</v>
       </c>
       <c r="C2">
-        <v>0.5087883898750433</v>
+        <v>0.50878838987504327</v>
       </c>
       <c r="D2">
-        <v>1.117831929593637E-08</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>1.1178319295936369E-8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B3">
-        <v>-0.02938514214215259</v>
+        <v>-2.9385142142152591E-2</v>
       </c>
       <c r="C3">
-        <v>0.01978078660547302</v>
+        <v>1.9780786605473021E-2</v>
       </c>
       <c r="D3">
-        <v>0.1403141549531085</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.14031415495310851</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B4">
-        <v>-0.03805872146715064</v>
+        <v>-3.8058721467150641E-2</v>
       </c>
       <c r="C4">
-        <v>0.06155972582955792</v>
+        <v>6.1559725829557918E-2</v>
       </c>
       <c r="D4">
-        <v>0.5377183905030244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>0.53771839050302439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B5">
-        <v>-0.5267503558328671</v>
+        <v>-0.52675035583286711</v>
       </c>
       <c r="C5">
-        <v>0.1681316328394694</v>
+        <v>0.16813163283946941</v>
       </c>
       <c r="D5">
-        <v>0.002227836944820977</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>2.2278369448209771E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>73</v>
       </c>
@@ -1819,10 +1884,10 @@
         <v>0.1236163437937919</v>
       </c>
       <c r="C6">
-        <v>0.1830485738301472</v>
+        <v>0.18304857383014719</v>
       </c>
       <c r="D6">
-        <v>0.5009158769473905</v>
+        <v>0.50091587694739048</v>
       </c>
     </row>
   </sheetData>
@@ -1831,14 +1896,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1849,63 +1914,63 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B2">
-        <v>3.193804128002517</v>
+        <v>3.1938041280025171</v>
       </c>
       <c r="C2">
-        <v>0.5159341169406552</v>
+        <v>0.51593411694065516</v>
       </c>
       <c r="D2">
-        <v>1.129195966357384E-08</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>1.1291959663573839E-8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B3">
-        <v>-0.03024446416596019</v>
+        <v>-3.0244464165960189E-2</v>
       </c>
       <c r="C3">
-        <v>0.01989147635850407</v>
+        <v>1.9891476358504068E-2</v>
       </c>
       <c r="D3">
-        <v>0.1313416111179284</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.13134161111792839</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B4">
-        <v>-0.03831655912785886</v>
+        <v>-3.8316559127858862E-2</v>
       </c>
       <c r="C4">
-        <v>0.06174467128090202</v>
+        <v>6.1744671280902018E-2</v>
       </c>
       <c r="D4">
-        <v>0.5362056771655552</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>0.53620567716555523</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B5">
-        <v>-0.5229478789328783</v>
+        <v>-0.52294787893287831</v>
       </c>
       <c r="C5">
-        <v>0.1687519731699423</v>
+        <v>0.16875197316994231</v>
       </c>
       <c r="D5">
-        <v>0.002481856545270264</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>2.481856545270264E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>75</v>
       </c>
@@ -1913,13 +1978,13 @@
         <v>-0.1114284982442931</v>
       </c>
       <c r="C6">
-        <v>0.1859233184765345</v>
+        <v>0.18592331847653451</v>
       </c>
       <c r="D6">
-        <v>0.5502230686172668</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>0.55022306861726678</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -1927,10 +1992,10 @@
         <v>0.1465672178519726</v>
       </c>
       <c r="C7">
-        <v>0.1875453235880244</v>
+        <v>0.18754532358802439</v>
       </c>
       <c r="D7">
-        <v>0.4362325596286328</v>
+        <v>0.43623255962863278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>